<commit_message>
removido arquivo de teste
</commit_message>
<xml_diff>
--- a/planilha/contatos.xlsx
+++ b/planilha/contatos.xlsx
@@ -146,10 +146,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
   </cols>
@@ -167,7 +167,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>5532988141424</v>
+        <v>5532999999999</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -175,7 +175,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>5532984943333</v>
+        <v>5532999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: adicionado tratamento de erro caso o navegador seja fechado
caso o usuario feche o navegador inesperadamente aparecerá mensagem de erro
</commit_message>
<xml_diff>
--- a/planilha/contatos.xlsx
+++ b/planilha/contatos.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Diogo</t>
   </si>
   <si>
-    <t xml:space="preserve">Flávio</t>
+    <t xml:space="preserve">Fulano</t>
   </si>
 </sst>
 </file>
@@ -41,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -69,6 +69,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,7 +118,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -123,6 +128,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -146,10 +155,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
   </cols>
@@ -174,7 +183,7 @@
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>5532999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(Diogo): adicionado tratamento de erros
adicionado tratamento de erros para todas as funções de envio de mensagem.

resolução card #1453
</commit_message>
<xml_diff>
--- a/planilha/contatos.xlsx
+++ b/planilha/contatos.xlsx
@@ -41,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -69,11 +69,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,7 +126,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,10 +150,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
   </cols>
@@ -176,7 +171,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>5532999999999</v>
+        <v>5532988141424</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -184,7 +179,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>5532999999999</v>
+        <v>5532988141424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>